<commit_message>
class AM 9:00 - 12:50
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ppt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03909BE4-2FC5-47C0-B006-7F02EE6CD163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8220AD-78C9-4822-BFB4-141258ACAC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="5775" windowWidth="12480" windowHeight="11385" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
+    <workbookView xWindow="5685" yWindow="3450" windowWidth="12480" windowHeight="11385" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
@@ -129,17 +129,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,17 +459,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643977C-A067-4C33-B0A8-658AE0A3A2A5}">
-  <dimension ref="B2:N24"/>
+  <dimension ref="B2:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.875" customWidth="1"/>
     <col min="2" max="2" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.125" customWidth="1"/>
     <col min="4" max="4" width="4.375" customWidth="1"/>
     <col min="5" max="11" width="3.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.75" bestFit="1" customWidth="1"/>
@@ -478,10 +481,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -489,18 +492,18 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
     </row>
@@ -510,28 +513,28 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L6" t="s">
@@ -607,7 +610,7 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>1</v>
       </c>
       <c r="N9">
@@ -633,7 +636,7 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10">
@@ -659,7 +662,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>1</v>
       </c>
       <c r="J11">
@@ -685,7 +688,7 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>1</v>
       </c>
       <c r="I12">
@@ -711,7 +714,7 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>1</v>
       </c>
       <c r="H13">
@@ -737,7 +740,7 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14">
@@ -763,7 +766,7 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15">
@@ -789,7 +792,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16">
@@ -995,6 +998,35 @@
       </c>
       <c r="N24">
         <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
organize folder and files. first step.
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ppt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8220AD-78C9-4822-BFB4-141258ACAC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B9044F-7607-4618-A356-792A4BCBDF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="3450" windowWidth="12480" windowHeight="11385" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
+    <workbookView xWindow="8760" yWindow="2685" windowWidth="10860" windowHeight="12930" activeTab="1" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
+    <sheet name="컴퓨터상식" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +72,12 @@
   <si>
     <t>십진수</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visual studio code : 대부분 언어 커버</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDE : 통합개발환경, integrated deveopment enviornment </t>
   </si>
 </sst>
 </file>
@@ -139,10 +146,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -461,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643977C-A067-4C33-B0A8-658AE0A3A2A5}">
   <dimension ref="B2:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:H27"/>
     </sheetView>
   </sheetViews>
@@ -481,10 +488,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -495,15 +502,15 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -516,25 +523,25 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L6" t="s">
@@ -545,16 +552,16 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
       <c r="N7" t="s">
         <v>11</v>
       </c>
@@ -1036,4 +1043,30 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5BDAE5-CBE5-487E-BD41-3E142EF656DB}">
+  <dimension ref="B2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AM 9:00 - 12:50 class
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ppt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DF85BD-7B3B-4D5B-93C1-14EC2F1D74EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629D8C51-DECE-44B3-9D1B-74DB29D263C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
+    <workbookView xWindow="2625" yWindow="930" windowWidth="16005" windowHeight="13455" activeTab="3" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
     <sheet name="컴퓨터상식" sheetId="2" r:id="rId2"/>
+    <sheet name="자료형" sheetId="3" r:id="rId3"/>
+    <sheet name="클래스" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,6 +178,405 @@
   <si>
     <t>16진수
 (hexadecimal)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># CPU : 산술 (Arithmetic), 논리 (Logical), 제어 (control Unit)  --- ALU</t>
+  </si>
+  <si>
+    <t># 클래스명 앞글자 : 대문자.</t>
+  </si>
+  <si>
+    <r>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E4E8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB392F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyword</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"># ['False', 'None:비어있다.', 'True', 'and', 'as', 'assert', 'async', 'await', 'break', 'class', 'continue', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#  'def', 'del', 'elif', 'else', 'except', 'finally', 'for', 'from', 'global', 'if', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#  'import', 'in', 'is', 'lambda', 'nonlocal', 'not', 'or', 'pass', </t>
+  </si>
+  <si>
+    <t>#  'raise','return', 'try', 'while', 'with', 'yield']</t>
+  </si>
+  <si>
+    <t># keyword는 라이브러리.</t>
+  </si>
+  <si>
+    <t>0을 제외한 나머지 참</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0이란 개념은 빈 것과 None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정수(int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실수(float)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불리언(True/False)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>keyword</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>kwlist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE1E4E8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>접근하다는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의미이다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF6A737D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특수문자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자로 시작 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공백 포함 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약어 사용 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변수설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">스네이크 케이스 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(snake case) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>언더바</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(_)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>기호 중간에 붙이기</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">캐멀 케이스 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(camel case) : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="4"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>단어들의 첫 글자를 대문자로 만들기</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">파이썬에서는 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>스네이크(파이썬에서 주로사용)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 및 캐멀 케이스 둘 모두 사용</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>느린이유? 파이썬은 Mapper를 한 번 감쌌다. 그래서 C언어보다 느리다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>붕어빵틀(클래스)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>붕어빵(객체)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클래스는 '틀'이자 '단위'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>객체는 틀(클래스)에서 찍은 놈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>object oriented program</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세상을 지배하는 프로그래밍 방법론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소프트웨어 공학</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -183,7 +584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +613,91 @@
       <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE1E4E8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A737D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF97583"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB392F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A737D"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="4"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -316,7 +802,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -332,47 +818,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -691,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643977C-A067-4C33-B0A8-658AE0A3A2A5}">
   <dimension ref="B2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -727,22 +1228,22 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <v>10</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="12">
         <v>11</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="12">
         <v>12</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="12">
         <v>13</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <v>14</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="12">
         <v>15</v>
       </c>
     </row>
@@ -753,22 +1254,22 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="S3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -818,16 +1319,16 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
       <c r="N7" t="s">
         <v>32</v>
       </c>
@@ -1306,34 +1807,34 @@
       <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="8">
-        <v>0</v>
-      </c>
-      <c r="D26" s="8">
-        <v>1</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="6">
-        <v>1</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="7">
-        <v>0</v>
-      </c>
-      <c r="J26" s="7">
-        <v>0</v>
-      </c>
-      <c r="K26" s="7">
-        <v>1</v>
-      </c>
-      <c r="L26" s="12">
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6">
+        <v>0</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
+        <v>1</v>
+      </c>
+      <c r="L26" s="11">
         <v>351</v>
       </c>
       <c r="N26">
@@ -1344,21 +1845,21 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="17">
         <v>3</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17">
         <v>5</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15">
-        <v>1</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17">
+        <v>1</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -1369,34 +1870,34 @@
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1</v>
-      </c>
-      <c r="F29" s="10">
-        <v>1</v>
-      </c>
-      <c r="G29" s="10">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
-        <v>1</v>
-      </c>
-      <c r="I29" s="9">
-        <v>0</v>
-      </c>
-      <c r="J29" s="9">
-        <v>0</v>
-      </c>
-      <c r="K29" s="9">
-        <v>1</v>
-      </c>
-      <c r="M29" s="11" t="s">
+      <c r="D29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
+      <c r="M29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="14">
+      <c r="N29">
         <v>233</v>
       </c>
     </row>
@@ -1404,18 +1905,18 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>9</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -1423,31 +1924,31 @@
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="E33" s="9">
-        <v>1</v>
-      </c>
-      <c r="F33" s="8">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8">
-        <v>1</v>
-      </c>
-      <c r="H33" s="8">
-        <v>1</v>
-      </c>
-      <c r="I33" s="16">
-        <v>0</v>
-      </c>
-      <c r="J33" s="16">
-        <v>1</v>
-      </c>
-      <c r="K33" s="16">
+      <c r="C33" s="8">
+        <v>0</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1</v>
+      </c>
+      <c r="I33" s="13">
+        <v>0</v>
+      </c>
+      <c r="J33" s="13">
+        <v>1</v>
+      </c>
+      <c r="K33" s="13">
         <v>0</v>
       </c>
       <c r="N33">
@@ -1458,45 +1959,45 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="17">
         <v>3</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15">
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17">
         <v>7</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15">
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17">
         <v>2</v>
       </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D35" s="7">
-        <v>1</v>
-      </c>
-      <c r="E35" s="7">
-        <v>1</v>
-      </c>
-      <c r="F35" s="7">
-        <v>1</v>
-      </c>
-      <c r="G35" s="7">
-        <v>1</v>
-      </c>
-      <c r="H35" s="17">
-        <v>1</v>
-      </c>
-      <c r="I35" s="17">
-        <v>0</v>
-      </c>
-      <c r="J35" s="17">
-        <v>1</v>
-      </c>
-      <c r="K35" s="17">
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+      <c r="H35" s="14">
+        <v>1</v>
+      </c>
+      <c r="I35" s="14">
+        <v>0</v>
+      </c>
+      <c r="J35" s="14">
+        <v>1</v>
+      </c>
+      <c r="K35" s="14">
         <v>0</v>
       </c>
       <c r="N35">
@@ -1504,21 +2005,21 @@
       </c>
     </row>
     <row r="36" spans="2:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15" t="s">
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1625,4 +2126,211 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C094A0-5954-4EC1-9E5B-5BF05ABDB40A}">
+  <dimension ref="B2:D29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B25" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B26" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A3DF72-F4DC-4410-9F57-CDEE8532AC1E}">
+  <dimension ref="B3:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
practice dictionary and sorting
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ppt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E2E3B-2C94-4B7D-B4CE-725D3B7C835B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD853A51-B76A-4470-972F-0164FF178BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="0" windowWidth="13680" windowHeight="17400" firstSheet="2" activeTab="7" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
+    <workbookView xWindow="-45" yWindow="60" windowWidth="13365" windowHeight="11100" firstSheet="2" activeTab="5" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -715,12 +715,56 @@
     <t>1500원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>값의 개수를 셀 때 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'a': [1,2,3,4…]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개수(value)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">값(key) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>값 swap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>값으 ㅣ개수 세는 알고리즘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">in </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>있냐없냐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찾고자 하는 값 in iterable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iterable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:리스트 , 문자열, 튜플, 딕셔너리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,8 +906,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,6 +983,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1083,7 +1148,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1156,37 +1221,46 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1858,16 +1932,16 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
       <c r="N7" t="s">
         <v>32</v>
       </c>
@@ -2384,21 +2458,21 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="34">
         <v>3</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25">
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34">
         <v>5</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25">
-        <v>1</v>
-      </c>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34">
+        <v>1</v>
+      </c>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -2444,18 +2518,18 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25">
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34">
         <v>9</v>
       </c>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -2498,21 +2572,21 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="34">
         <v>3</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25">
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34">
         <v>7</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25">
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34">
         <v>2</v>
       </c>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D35" s="6">
@@ -2547,18 +2621,18 @@
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25" t="s">
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2671,8 +2745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C094A0-5954-4EC1-9E5B-5BF05ABDB40A}">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2823,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A3DF72-F4DC-4410-9F57-CDEE8532AC1E}">
   <dimension ref="B3:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2943,10 +3017,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5742511C-F6C2-4D8F-AD8F-0806C110200B}">
-  <dimension ref="B2:H7"/>
+  <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2954,15 +3028,17 @@
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
     <col min="8" max="8" width="9.625" customWidth="1"/>
+    <col min="12" max="12" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>50</v>
       </c>
@@ -2970,7 +3046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>92</v>
       </c>
@@ -2981,7 +3057,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>93</v>
       </c>
@@ -2992,7 +3068,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E6" s="23" t="s">
         <v>88</v>
       </c>
@@ -3000,15 +3076,62 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E7" s="23" t="s">
         <v>90</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>91</v>
       </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K9" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K9:L9"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3034,7 +3157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD498B0-A2E8-4118-BE41-F31E68278A6C}">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3042,66 +3165,66 @@
   <sheetData>
     <row r="2" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="30">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="30">
+      <c r="B6" s="28">
         <v>3</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
solve problem ppt 04-03
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\ppt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD853A51-B76A-4470-972F-0164FF178BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BB7D11-E06F-4167-A3FC-3FE862FA3003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="60" windowWidth="13365" windowHeight="11100" firstSheet="2" activeTab="5" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18180" windowHeight="13035" firstSheet="6" activeTab="9" xr2:uid="{C292E0BC-00EB-4779-A60C-E007E6A4F4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
     <sheet name="컴퓨터상식" sheetId="2" r:id="rId2"/>
     <sheet name="자료형" sheetId="3" r:id="rId3"/>
-    <sheet name="클래스" sheetId="4" r:id="rId4"/>
-    <sheet name="문자열" sheetId="5" r:id="rId5"/>
-    <sheet name="자료구조" sheetId="6" r:id="rId6"/>
-    <sheet name="쿠팡홈페이지_이미지" sheetId="7" r:id="rId7"/>
-    <sheet name="테이블연습" sheetId="8" r:id="rId8"/>
+    <sheet name="연산자" sheetId="9" r:id="rId4"/>
+    <sheet name="클래스" sheetId="4" r:id="rId5"/>
+    <sheet name="문자열" sheetId="5" r:id="rId6"/>
+    <sheet name="자료구조_알고리즘" sheetId="6" r:id="rId7"/>
+    <sheet name="쿠팡홈페이지_이미지" sheetId="7" r:id="rId8"/>
+    <sheet name="테이블연습" sheetId="8" r:id="rId9"/>
+    <sheet name="반복문" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="198">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -758,6 +761,257 @@
   <si>
     <t>:리스트 , 문자열, 튜플, 딕셔너리</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># -------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t># 순서 정렬하기</t>
+  </si>
+  <si>
+    <t>numbers = [1,2,6,8,4,3,2,1,9,5,4,9,7,2,1,3,5,4,8,9,7,2,3]</t>
+  </si>
+  <si>
+    <t>counter = {}</t>
+  </si>
+  <si>
+    <t>for number in numbers:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if bool(counter) == False :        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        counter[number] = 1        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else :         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if number in counter.keys():                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            counter[number] += 1   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        else :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            counter[number] = 1 </t>
+  </si>
+  <si>
+    <t>li = list(counter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">li.sort() </t>
+  </si>
+  <si>
+    <t>print("정렬 전:", counter)</t>
+  </si>
+  <si>
+    <t>result=dict(sorted(counter.items()))</t>
+  </si>
+  <si>
+    <t>print("정렬 후:", result)</t>
+  </si>
+  <si>
+    <t># # 밑의 코드와 같은 결과가 나온다. Counter Class 사용</t>
+  </si>
+  <si>
+    <t># # import collections</t>
+  </si>
+  <si>
+    <t># # print(collections.Counter(numbers))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>==</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>값이 같냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나머지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">a is b </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소값이 같냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; a is b</t>
+  </si>
+  <si>
+    <t># True</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; type(4) is int</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; type(True) is bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># &gt;&gt;&gt; type("string") is str </t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; type({'1':'223'}) is dict</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; type((1, 455435)) is tuple</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; type([1,'3434',True]) is list</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; a=5</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; b=5</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; a == b</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; id(a)</t>
+  </si>
+  <si>
+    <t># 140730768155560</t>
+  </si>
+  <si>
+    <t># &gt;&gt;&gt; id(b)</t>
+  </si>
+  <si>
+    <t># # 주소값이 a,b가 같냐?? 256 값 넘어가면 변수 주소값이 달라진다.</t>
+  </si>
+  <si>
+    <t>트리만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str1= ''</t>
+  </si>
+  <si>
+    <t>for i in range(1, 7):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for j in range(6, i, -1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        str1 += ' '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for k in range(0 , 2*i-1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        str1 += '*'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    str1 += '\n'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>for i in range(2):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for j in range(4):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for k in range(3):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        str1 += "*"</t>
+  </si>
+  <si>
+    <t>print(str1)</t>
+  </si>
+  <si>
+    <t># result : 1,3,5,7,9,11</t>
+  </si>
+  <si>
+    <t>import time</t>
+  </si>
+  <si>
+    <t>print("로켓 발사 카운드 다운")</t>
+  </si>
+  <si>
+    <t>for i in range(5, -1, -1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print(i)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    time.sleep(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for i in range(7):    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    result = 2*i+1            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for j in range(11+1):     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if j == result:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            space = int((11-result)//2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            print(" "*space + "*"*j)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            continue  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">for x in range(1, 2+1):    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print(" "*3, "*"*3)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">print("로 켓 발 사 !!")     </t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1402,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1248,6 +1502,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1256,12 +1522,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1932,16 +2192,16 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
       <c r="N7" t="s">
         <v>32</v>
       </c>
@@ -2458,21 +2718,21 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="38">
         <v>3</v>
       </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34">
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38">
         <v>5</v>
       </c>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34">
-        <v>1</v>
-      </c>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38">
+        <v>1</v>
+      </c>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -2518,18 +2778,18 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34">
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38">
         <v>9</v>
       </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -2572,21 +2832,21 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="38">
         <v>3</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34">
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38">
         <v>7</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34">
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38">
         <v>2</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D35" s="6">
@@ -2621,18 +2881,18 @@
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34" t="s">
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2648,6 +2908,211 @@
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="F27:H27"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662AAAFD-E456-4291-812C-7A0F7F9D2F83}">
+  <dimension ref="B4:B45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F46577B-A38D-4F2F-8D0B-4F45FAE04A69}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2894,6 +3359,236 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE7CA56-6260-453E-899E-D0485F695165}">
+  <dimension ref="B2:C46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="36"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="36"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="36"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="36"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A3DF72-F4DC-4410-9F57-CDEE8532AC1E}">
   <dimension ref="B3:I9"/>
   <sheetViews>
@@ -2945,7 +3640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA76733-CB72-4885-B631-B5DFB7B67C2C}">
   <dimension ref="B2:D11"/>
   <sheetViews>
@@ -3015,12 +3710,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5742511C-F6C2-4D8F-AD8F-0806C110200B}">
-  <dimension ref="B2:L18"/>
+  <dimension ref="B2:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3088,18 +3783,18 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L8" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="35"/>
+      <c r="L9" s="39"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -3112,10 +3807,10 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="34" t="s">
         <v>115</v>
       </c>
       <c r="H18" t="s">
@@ -3126,6 +3821,121 @@
       </c>
       <c r="L18" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3137,7 +3947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A05455-5B8A-4366-A5B2-21DF9A535D3E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3153,12 +3963,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD498B0-A2E8-4118-BE41-F31E68278A6C}">
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update symentic tag and html
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14445" windowHeight="16080" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="14445" windowHeight="16080" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="쿠팡홈페이지_이미지" sheetId="7" r:id="rId8"/>
     <sheet name="테이블연습" sheetId="8" r:id="rId9"/>
     <sheet name="반복문" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId11"/>
+    <sheet name="함수" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="282">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1251,6 +1251,30 @@
   </si>
   <si>
     <t># 딕셔너리.items()</t>
+  </si>
+  <si>
+    <t>scope룰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변수의 사용 범위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변수가 코드에서 사용되는 범위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변수의 사용범위를 고려해야 될 2가지'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 지역변수(local variable) : 함수 내에서만 사용가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 전역변수(global variable) : 프로그램 전체에서만 사용가능.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1647,7 +1671,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1759,6 +1783,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1768,7 +1795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2440,16 +2467,16 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
       <c r="N7" t="s">
         <v>32</v>
       </c>
@@ -2966,21 +2993,21 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="39">
         <v>3</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38">
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39">
         <v>5</v>
       </c>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38">
-        <v>1</v>
-      </c>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39">
+        <v>1</v>
+      </c>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -3026,18 +3053,18 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38">
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39">
         <v>9</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -3080,21 +3107,21 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="39">
         <v>3</v>
       </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38">
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39">
         <v>7</v>
       </c>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38">
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39">
         <v>2</v>
       </c>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D35" s="6">
@@ -3129,18 +3156,18 @@
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38" t="s">
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3355,12 +3382,48 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3962,8 +4025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123:H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4039,10 +4102,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="K9" s="39" t="s">
+      <c r="K9" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="39"/>
+      <c r="L9" s="40"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -4187,22 +4250,22 @@
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="37" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="37" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="37" t="s">
         <v>275</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save image and lambda conception.
</commit_message>
<xml_diff>
--- a/ppt2/통합수업자료_shjung.xlsx
+++ b/ppt2/통합수업자료_shjung.xlsx
@@ -9,24 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14445" windowHeight="16080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="14445" windowHeight="16080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="비트_240715" sheetId="1" r:id="rId1"/>
     <sheet name="그리스문자" sheetId="14" r:id="rId2"/>
     <sheet name="데이터타입(자료형)" sheetId="15" r:id="rId3"/>
-    <sheet name="컴퓨터상식" sheetId="2" r:id="rId4"/>
-    <sheet name="자료형" sheetId="3" r:id="rId5"/>
-    <sheet name="연산자" sheetId="9" r:id="rId6"/>
-    <sheet name="클래스" sheetId="4" r:id="rId7"/>
-    <sheet name="문자열" sheetId="5" r:id="rId8"/>
-    <sheet name="자료구조_알고리즘" sheetId="6" r:id="rId9"/>
-    <sheet name="쿠팡홈페이지_이미지" sheetId="7" r:id="rId10"/>
-    <sheet name="테이블연습" sheetId="8" r:id="rId11"/>
-    <sheet name="반복문" sheetId="10" r:id="rId12"/>
-    <sheet name="함수" sheetId="11" r:id="rId13"/>
-    <sheet name="기초수학" sheetId="12" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="13" r:id="rId15"/>
+    <sheet name="그래프양식1" sheetId="16" r:id="rId4"/>
+    <sheet name="컴퓨터상식" sheetId="2" r:id="rId5"/>
+    <sheet name="자료형" sheetId="3" r:id="rId6"/>
+    <sheet name="연산자" sheetId="9" r:id="rId7"/>
+    <sheet name="클래스" sheetId="4" r:id="rId8"/>
+    <sheet name="문자열" sheetId="5" r:id="rId9"/>
+    <sheet name="자료구조_알고리즘" sheetId="6" r:id="rId10"/>
+    <sheet name="쿠팡홈페이지_이미지" sheetId="7" r:id="rId11"/>
+    <sheet name="테이블연습" sheetId="8" r:id="rId12"/>
+    <sheet name="반복문" sheetId="10" r:id="rId13"/>
+    <sheet name="함수" sheetId="11" r:id="rId14"/>
+    <sheet name="기초수학" sheetId="12" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="513">
   <si>
     <t>bit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2154,6 +2155,90 @@
   </si>
   <si>
     <t>{} 연관배열(hashtable)</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=ax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-1x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=-ax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=-x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=-2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=-3x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=1x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=3x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=1x+3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=1x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=1x-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2556,7 +2641,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2699,6 +2784,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2708,7 +2822,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2862,13 +2976,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2901,20 +3009,11 @@
     <xf numFmtId="0" fontId="35" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2925,19 +3024,10 @@
     <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2949,9 +3039,6 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2961,14 +3048,62 @@
     <xf numFmtId="0" fontId="31" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3049,6 +3184,432 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7328</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="직선 연결선 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="285751" y="652097"/>
+          <a:ext cx="2798884" cy="1633903"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>249115</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>175847</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="직선 연결선 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="586153" y="432289"/>
+          <a:ext cx="2168770" cy="2080846"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>109904</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>153865</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="직선 연결선 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="945173" y="190501"/>
+          <a:ext cx="1436077" cy="2601057"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219807</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="직선 연결선 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="498230" y="3722077"/>
+          <a:ext cx="2381250" cy="2359270"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>159728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>73269</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="직선 연결선 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="4409343"/>
+          <a:ext cx="2888273" cy="961291"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>117231</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161193</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="직선 연결선 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="3678116"/>
+          <a:ext cx="1582615" cy="2645019"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>197829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>36634</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>131884</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="직선 연결선 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="21981" y="7209694"/>
+          <a:ext cx="2798884" cy="1633902"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>263769</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>29309</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>278422</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="직선 연결선 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="263769" y="7678617"/>
+          <a:ext cx="2798884" cy="1633902"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66138</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>206497</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>65942</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>131885</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="직선 연결선 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="344561" y="8280766"/>
+          <a:ext cx="2784035" cy="1625234"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3273,7 +3834,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3856,16 +4417,16 @@
       </c>
     </row>
     <row r="7" spans="2:20">
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
       <c r="N7" t="s">
         <v>32</v>
       </c>
@@ -4382,21 +4943,21 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="77">
         <v>3</v>
       </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52">
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77">
         <v>5</v>
       </c>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52">
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77">
         <v>1</v>
       </c>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" t="s">
@@ -4442,18 +5003,18 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52">
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77">
         <v>9</v>
       </c>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" t="s">
@@ -4496,21 +5057,21 @@
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="52">
+      <c r="C34" s="77">
         <v>3</v>
       </c>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52">
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77">
         <v>7</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52">
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77">
         <v>2</v>
       </c>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="2:14">
       <c r="D35" s="6">
@@ -4545,18 +5106,18 @@
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52" t="s">
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="52"/>
-      <c r="J36" s="52"/>
-      <c r="K36" s="52"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4579,6 +5140,676 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L149"/>
+  <sheetViews>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123:H124"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
+    <col min="8" max="8" width="9.625" customWidth="1"/>
+    <col min="12" max="12" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="E6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="E7" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="K8" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="K9" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="87"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="5" customFormat="1">
+      <c r="B24" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" s="5" customFormat="1">
+      <c r="B25" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" s="5" customFormat="1">
+      <c r="B26" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="37" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="37" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="37" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12">
+      <c r="B56" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="B58" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="B60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12">
+      <c r="B61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12">
+      <c r="B64" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" s="5" customFormat="1">
+      <c r="B76" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" s="5" customFormat="1">
+      <c r="B89" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" s="5" customFormat="1">
+      <c r="B113" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" s="5" customFormat="1">
+      <c r="B135" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K9:L9"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -4593,7 +5824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E7"/>
   <sheetViews>
@@ -4673,7 +5904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:B45"/>
   <sheetViews>
@@ -4865,7 +6096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
@@ -4914,7 +6145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z78"/>
   <sheetViews>
@@ -5369,7 +6600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5402,7 +6633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -5430,7 +6661,7 @@
       <c r="P1" s="44"/>
       <c r="Q1" s="44"/>
       <c r="R1" s="44"/>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="52" t="s">
         <v>328</v>
       </c>
       <c r="T1" s="44"/>
@@ -5551,13 +6782,13 @@
       <c r="N4" s="44"/>
       <c r="O4" s="44"/>
       <c r="P4" s="44"/>
-      <c r="Q4" s="55" t="s">
+      <c r="Q4" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="R4" s="55" t="s">
+      <c r="R4" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="S4" s="55" t="s">
+      <c r="S4" s="53" t="s">
         <v>339</v>
       </c>
       <c r="T4" s="44"/>
@@ -5594,31 +6825,31 @@
       <c r="H5" s="44" t="s">
         <v>344</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="53" t="s">
         <v>345</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="53" t="s">
         <v>346</v>
       </c>
       <c r="O5" s="44"/>
       <c r="P5" s="44"/>
-      <c r="Q5" s="55" t="s">
+      <c r="Q5" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="R5" s="56" t="s">
+      <c r="R5" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="S5" s="55">
+      <c r="S5" s="53">
         <v>1</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="U5" s="57">
+      <c r="U5" s="55">
         <v>-128</v>
       </c>
       <c r="V5" s="46">
@@ -5658,16 +6889,16 @@
       <c r="Q6" s="44" t="s">
         <v>348</v>
       </c>
-      <c r="R6" s="56" t="s">
+      <c r="R6" s="54" t="s">
         <v>349</v>
       </c>
-      <c r="S6" s="55">
+      <c r="S6" s="53">
         <v>2</v>
       </c>
-      <c r="T6" s="57" t="s">
+      <c r="T6" s="55" t="s">
         <v>350</v>
       </c>
-      <c r="U6" s="57">
+      <c r="U6" s="55">
         <v>-32768</v>
       </c>
       <c r="V6" s="46">
@@ -5700,34 +6931,34 @@
       <c r="H7" s="44" t="s">
         <v>352</v>
       </c>
-      <c r="I7" s="55">
+      <c r="I7" s="53">
         <f>-2 -1</f>
         <v>-3</v>
       </c>
-      <c r="J7" s="55">
+      <c r="J7" s="53">
         <v>0</v>
       </c>
-      <c r="K7" s="55" t="s">
+      <c r="K7" s="53" t="s">
         <v>353</v>
       </c>
       <c r="L7" s="44"/>
       <c r="M7" s="44"/>
-      <c r="N7" s="58" t="s">
+      <c r="N7" s="56" t="s">
         <v>354</v>
       </c>
       <c r="O7" s="44"/>
       <c r="P7" s="44"/>
       <c r="Q7" s="44"/>
-      <c r="R7" s="56" t="s">
+      <c r="R7" s="54" t="s">
         <v>355</v>
       </c>
-      <c r="S7" s="55">
+      <c r="S7" s="53">
         <v>4</v>
       </c>
-      <c r="T7" s="57" t="s">
+      <c r="T7" s="55" t="s">
         <v>356</v>
       </c>
-      <c r="U7" s="57">
+      <c r="U7" s="55">
         <v>-2147483648</v>
       </c>
       <c r="V7" s="46">
@@ -5765,13 +6996,13 @@
       <c r="O8" s="44"/>
       <c r="P8" s="44"/>
       <c r="Q8" s="44"/>
-      <c r="R8" s="56" t="s">
+      <c r="R8" s="54" t="s">
         <v>357</v>
       </c>
-      <c r="S8" s="55">
+      <c r="S8" s="53">
         <v>8</v>
       </c>
-      <c r="T8" s="57" t="s">
+      <c r="T8" s="55" t="s">
         <v>358</v>
       </c>
       <c r="U8" s="44"/>
@@ -5799,21 +7030,21 @@
       <c r="H9" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="I9" s="59">
+      <c r="I9" s="57">
         <v>3.4</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="44"/>
       <c r="M9" s="44"/>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="58" t="s">
         <v>360</v>
       </c>
       <c r="O9" s="45" t="s">
         <v>361</v>
       </c>
       <c r="P9" s="44"/>
-      <c r="Q9" s="55" t="s">
+      <c r="Q9" s="53" t="s">
         <v>362</v>
       </c>
       <c r="R9" s="40"/>
@@ -5849,7 +7080,7 @@
       <c r="K10" s="44"/>
       <c r="L10" s="44"/>
       <c r="M10" s="44"/>
-      <c r="N10" s="61" t="s">
+      <c r="N10" s="59" t="s">
         <v>363</v>
       </c>
       <c r="O10" s="45" t="s">
@@ -5857,13 +7088,13 @@
       </c>
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
-      <c r="R10" s="56" t="s">
+      <c r="R10" s="54" t="s">
         <v>362</v>
       </c>
-      <c r="S10" s="55">
+      <c r="S10" s="53">
         <v>4</v>
       </c>
-      <c r="T10" s="57" t="s">
+      <c r="T10" s="55" t="s">
         <v>365</v>
       </c>
       <c r="U10" s="44"/>
@@ -5900,13 +7131,13 @@
       <c r="O11" s="44"/>
       <c r="P11" s="44"/>
       <c r="Q11" s="44"/>
-      <c r="R11" s="56" t="s">
+      <c r="R11" s="54" t="s">
         <v>366</v>
       </c>
-      <c r="S11" s="55">
+      <c r="S11" s="53">
         <v>8</v>
       </c>
-      <c r="T11" s="57" t="s">
+      <c r="T11" s="55" t="s">
         <v>367</v>
       </c>
       <c r="U11" s="44"/>
@@ -5976,16 +7207,16 @@
       <c r="O13" s="44"/>
       <c r="P13" s="44"/>
       <c r="Q13" s="44"/>
-      <c r="R13" s="56" t="s">
+      <c r="R13" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="S13" s="55">
+      <c r="S13" s="53">
         <v>2</v>
       </c>
-      <c r="T13" s="57" t="s">
+      <c r="T13" s="55" t="s">
         <v>369</v>
       </c>
-      <c r="U13" s="57">
+      <c r="U13" s="55">
         <v>65536</v>
       </c>
       <c r="V13" s="44" t="s">
@@ -6008,7 +7239,7 @@
       <c r="B14" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="60" t="s">
         <v>372</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -6029,13 +7260,13 @@
       <c r="O14" s="44"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="44"/>
-      <c r="R14" s="56" t="s">
+      <c r="R14" s="54" t="s">
         <v>375</v>
       </c>
-      <c r="S14" s="55">
+      <c r="S14" s="53">
         <v>1</v>
       </c>
-      <c r="T14" s="57" t="s">
+      <c r="T14" s="55" t="s">
         <v>347</v>
       </c>
       <c r="U14" s="44"/>
@@ -6107,7 +7338,7 @@
       <c r="K16" s="44"/>
       <c r="L16" s="44"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="63" t="s">
+      <c r="N16" s="61" t="s">
         <v>379</v>
       </c>
       <c r="O16" s="44"/>
@@ -6251,7 +7482,7 @@
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
-      <c r="N20" s="55" t="s">
+      <c r="N20" s="53" t="s">
         <v>381</v>
       </c>
       <c r="O20" s="45" t="s">
@@ -7203,10 +8434,10 @@
       <c r="E46" s="44"/>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="81" t="s">
         <v>403</v>
       </c>
-      <c r="I46" s="64"/>
+      <c r="I46" s="81"/>
       <c r="J46" s="44"/>
       <c r="K46" s="44"/>
       <c r="L46" s="44"/>
@@ -7240,10 +8471,10 @@
       <c r="E47" s="44"/>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
-      <c r="H47" s="55" t="s">
+      <c r="H47" s="53" t="s">
         <v>404</v>
       </c>
-      <c r="I47" s="55" t="s">
+      <c r="I47" s="53" t="s">
         <v>405</v>
       </c>
       <c r="J47" s="44"/>
@@ -7279,10 +8510,10 @@
       <c r="E48" s="44"/>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
-      <c r="H48" s="56" t="s">
+      <c r="H48" s="54" t="s">
         <v>406</v>
       </c>
-      <c r="I48" s="56" t="s">
+      <c r="I48" s="54" t="s">
         <v>407</v>
       </c>
       <c r="J48" s="45" t="s">
@@ -7403,7 +8634,7 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
       <c r="P51" s="44"/>
-      <c r="Q51" s="54" t="s">
+      <c r="Q51" s="52" t="s">
         <v>411</v>
       </c>
       <c r="R51" s="44"/>
@@ -7441,7 +8672,7 @@
       <c r="O52" s="44"/>
       <c r="P52" s="44"/>
       <c r="Q52" s="44"/>
-      <c r="R52" s="54" t="s">
+      <c r="R52" s="52" t="s">
         <v>412</v>
       </c>
       <c r="S52" s="44"/>
@@ -7466,10 +8697,10 @@
         <v>413</v>
       </c>
       <c r="C53" s="44"/>
-      <c r="D53" s="65" t="s">
+      <c r="D53" s="62" t="s">
         <v>414</v>
       </c>
-      <c r="E53" s="65" t="s">
+      <c r="E53" s="62" t="s">
         <v>415</v>
       </c>
       <c r="F53" s="44"/>
@@ -7488,7 +8719,7 @@
       <c r="O53" s="44"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="44"/>
-      <c r="R53" s="54" t="s">
+      <c r="R53" s="52" t="s">
         <v>418</v>
       </c>
       <c r="S53" s="44"/>
@@ -7511,10 +8742,10 @@
       <c r="A54" s="44"/>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
-      <c r="D54" s="65" t="s">
+      <c r="D54" s="62" t="s">
         <v>419</v>
       </c>
-      <c r="E54" s="65" t="s">
+      <c r="E54" s="62" t="s">
         <v>420</v>
       </c>
       <c r="F54" s="44"/>
@@ -7530,7 +8761,7 @@
       <c r="N54" s="44"/>
       <c r="O54" s="44"/>
       <c r="P54" s="44"/>
-      <c r="Q54" s="54" t="s">
+      <c r="Q54" s="52" t="s">
         <v>422</v>
       </c>
       <c r="R54" s="44"/>
@@ -7556,10 +8787,10 @@
       <c r="C55" s="44" t="s">
         <v>423</v>
       </c>
-      <c r="D55" s="65" t="s">
+      <c r="D55" s="62" t="s">
         <v>424</v>
       </c>
-      <c r="E55" s="65" t="s">
+      <c r="E55" s="62" t="s">
         <v>425</v>
       </c>
       <c r="F55" s="44"/>
@@ -7573,7 +8804,7 @@
       <c r="N55" s="44"/>
       <c r="O55" s="44"/>
       <c r="P55" s="44"/>
-      <c r="Q55" s="55" t="s">
+      <c r="Q55" s="53" t="s">
         <v>426</v>
       </c>
       <c r="R55" s="44"/>
@@ -7611,7 +8842,7 @@
       <c r="O56" s="44"/>
       <c r="P56" s="44"/>
       <c r="Q56" s="44"/>
-      <c r="R56" s="55" t="s">
+      <c r="R56" s="53" t="s">
         <v>427</v>
       </c>
       <c r="S56" s="44"/>
@@ -7651,7 +8882,7 @@
       <c r="P57" s="44"/>
       <c r="Q57" s="44"/>
       <c r="R57" s="44"/>
-      <c r="S57" s="55" t="s">
+      <c r="S57" s="53" t="s">
         <v>429</v>
       </c>
       <c r="T57" s="44"/>
@@ -7725,7 +8956,7 @@
       <c r="P59" s="44"/>
       <c r="Q59" s="44"/>
       <c r="R59" s="44"/>
-      <c r="S59" s="55" t="s">
+      <c r="S59" s="53" t="s">
         <v>431</v>
       </c>
       <c r="T59" s="44"/>
@@ -7761,7 +8992,7 @@
       <c r="O60" s="44"/>
       <c r="P60" s="44"/>
       <c r="Q60" s="44"/>
-      <c r="R60" s="55" t="s">
+      <c r="R60" s="53" t="s">
         <v>432</v>
       </c>
       <c r="S60" s="44"/>
@@ -7798,7 +9029,7 @@
       <c r="O61" s="44"/>
       <c r="P61" s="44"/>
       <c r="Q61" s="44"/>
-      <c r="R61" s="54" t="s">
+      <c r="R61" s="52" t="s">
         <v>433</v>
       </c>
       <c r="S61" s="44"/>
@@ -7835,7 +9066,7 @@
       <c r="O62" s="44"/>
       <c r="P62" s="44"/>
       <c r="Q62" s="44"/>
-      <c r="R62" s="54" t="s">
+      <c r="R62" s="52" t="s">
         <v>434</v>
       </c>
       <c r="S62" s="44"/>
@@ -7872,7 +9103,7 @@
       <c r="O63" s="44"/>
       <c r="P63" s="44"/>
       <c r="Q63" s="44"/>
-      <c r="R63" s="54" t="s">
+      <c r="R63" s="52" t="s">
         <v>435</v>
       </c>
       <c r="S63" s="44"/>
@@ -7908,7 +9139,7 @@
       <c r="N64" s="44"/>
       <c r="O64" s="44"/>
       <c r="P64" s="44"/>
-      <c r="Q64" s="55" t="s">
+      <c r="Q64" s="53" t="s">
         <v>436</v>
       </c>
       <c r="R64" s="44"/>
@@ -8037,30 +9268,30 @@
     </row>
     <row r="68" spans="1:33" ht="30" customHeight="1">
       <c r="A68" s="40"/>
-      <c r="B68" s="66" t="s">
+      <c r="B68" s="63" t="s">
         <v>438</v>
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="40"/>
-      <c r="E68" s="67" t="s">
+      <c r="E68" s="82" t="s">
         <v>439</v>
       </c>
-      <c r="F68" s="67"/>
+      <c r="F68" s="82"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
-      <c r="I68" s="68" t="s">
+      <c r="I68" s="83" t="s">
         <v>440</v>
       </c>
-      <c r="J68" s="68"/>
-      <c r="K68" s="69" t="b">
+      <c r="J68" s="83"/>
+      <c r="K68" s="64" t="b">
         <v>0</v>
       </c>
       <c r="L68" s="40"/>
-      <c r="M68" s="67" t="s">
+      <c r="M68" s="82" t="s">
         <v>441</v>
       </c>
-      <c r="N68" s="67"/>
-      <c r="O68" s="67"/>
+      <c r="N68" s="82"/>
+      <c r="O68" s="82"/>
       <c r="P68" s="40"/>
       <c r="Q68" s="40"/>
       <c r="R68" s="40"/>
@@ -8089,24 +9320,24 @@
       <c r="F69" s="40"/>
       <c r="G69" s="40"/>
       <c r="H69" s="40"/>
-      <c r="I69" s="70" t="s">
+      <c r="I69" s="65" t="s">
         <v>442</v>
       </c>
-      <c r="J69" s="69" t="s">
+      <c r="J69" s="64" t="s">
         <v>443</v>
       </c>
-      <c r="K69" s="66" t="s">
+      <c r="K69" s="63" t="s">
         <v>442</v>
       </c>
       <c r="L69" s="40"/>
-      <c r="M69" s="69" t="s">
+      <c r="M69" s="64" t="s">
         <v>444</v>
       </c>
       <c r="N69" s="40"/>
-      <c r="O69" s="69" t="s">
+      <c r="O69" s="64" t="s">
         <v>445</v>
       </c>
-      <c r="P69" s="71" t="s">
+      <c r="P69" s="66" t="s">
         <v>446</v>
       </c>
       <c r="Q69" s="40"/>
@@ -8131,26 +9362,26 @@
       <c r="A70" s="44"/>
       <c r="B70" s="44"/>
       <c r="C70" s="44"/>
-      <c r="D70" s="72" t="s">
+      <c r="D70" s="80" t="s">
         <v>447</v>
       </c>
-      <c r="E70" s="73"/>
-      <c r="F70" s="74" t="s">
+      <c r="E70" s="67"/>
+      <c r="F70" s="68" t="s">
         <v>346</v>
       </c>
       <c r="G70" s="44"/>
       <c r="H70" s="44"/>
-      <c r="I70" s="75" t="s">
+      <c r="I70" s="84" t="s">
         <v>448</v>
       </c>
-      <c r="J70" s="76" t="s">
+      <c r="J70" s="85" t="s">
         <v>449</v>
       </c>
-      <c r="K70" s="77" t="s">
+      <c r="K70" s="69" t="s">
         <v>450</v>
       </c>
       <c r="L70" s="44"/>
-      <c r="M70" s="72" t="s">
+      <c r="M70" s="80" t="s">
         <v>451</v>
       </c>
       <c r="N70" s="44"/>
@@ -8178,20 +9409,20 @@
       <c r="A71" s="44"/>
       <c r="B71" s="44"/>
       <c r="C71" s="44"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="73"/>
-      <c r="F71" s="74" t="s">
+      <c r="D71" s="80"/>
+      <c r="E71" s="67"/>
+      <c r="F71" s="68" t="s">
         <v>349</v>
       </c>
       <c r="G71" s="44"/>
       <c r="H71" s="44"/>
-      <c r="I71" s="75"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="77" t="s">
+      <c r="I71" s="84"/>
+      <c r="J71" s="85"/>
+      <c r="K71" s="69" t="s">
         <v>452</v>
       </c>
       <c r="L71" s="44"/>
-      <c r="M71" s="72"/>
+      <c r="M71" s="80"/>
       <c r="N71" s="44"/>
       <c r="O71" s="44"/>
       <c r="P71" s="44"/>
@@ -8217,25 +9448,25 @@
       <c r="A72" s="44"/>
       <c r="B72" s="44"/>
       <c r="C72" s="44"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="78" t="s">
+      <c r="D72" s="80"/>
+      <c r="E72" s="70" t="s">
         <v>453</v>
       </c>
-      <c r="F72" s="74" t="s">
+      <c r="F72" s="68" t="s">
         <v>355</v>
       </c>
       <c r="G72" s="44"/>
       <c r="H72" s="44"/>
-      <c r="I72" s="75"/>
-      <c r="J72" s="76"/>
+      <c r="I72" s="84"/>
+      <c r="J72" s="85"/>
       <c r="K72" s="44"/>
       <c r="L72" s="44"/>
-      <c r="M72" s="72"/>
+      <c r="M72" s="80"/>
       <c r="N72" s="44"/>
-      <c r="O72" s="77" t="s">
+      <c r="O72" s="69" t="s">
         <v>454</v>
       </c>
-      <c r="P72" s="77" t="s">
+      <c r="P72" s="69" t="s">
         <v>454</v>
       </c>
       <c r="Q72" s="44"/>
@@ -8260,28 +9491,28 @@
       <c r="A73" s="44"/>
       <c r="B73" s="44"/>
       <c r="C73" s="44"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="73"/>
-      <c r="F73" s="74" t="s">
+      <c r="D73" s="80"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="68" t="s">
         <v>357</v>
       </c>
       <c r="G73" s="44"/>
       <c r="H73" s="44"/>
-      <c r="I73" s="75"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="77" t="s">
+      <c r="I73" s="84"/>
+      <c r="J73" s="85"/>
+      <c r="K73" s="69" t="s">
         <v>455</v>
       </c>
       <c r="L73" s="44"/>
-      <c r="M73" s="72"/>
+      <c r="M73" s="80"/>
       <c r="N73" s="44"/>
-      <c r="O73" s="77" t="s">
+      <c r="O73" s="69" t="s">
         <v>456</v>
       </c>
-      <c r="P73" s="77" t="s">
+      <c r="P73" s="69" t="s">
         <v>456</v>
       </c>
-      <c r="Q73" s="79" t="s">
+      <c r="Q73" s="71" t="s">
         <v>457</v>
       </c>
       <c r="R73" s="44"/>
@@ -8305,21 +9536,21 @@
       <c r="A74" s="44"/>
       <c r="B74" s="44"/>
       <c r="C74" s="44"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="73"/>
-      <c r="F74" s="73"/>
+      <c r="D74" s="80"/>
+      <c r="E74" s="67"/>
+      <c r="F74" s="67"/>
       <c r="G74" s="44"/>
       <c r="H74" s="44"/>
-      <c r="I74" s="75"/>
-      <c r="J74" s="76"/>
+      <c r="I74" s="84"/>
+      <c r="J74" s="85"/>
       <c r="K74" s="44"/>
       <c r="L74" s="44"/>
-      <c r="M74" s="72"/>
+      <c r="M74" s="80"/>
       <c r="N74" s="44"/>
-      <c r="O74" s="77" t="s">
+      <c r="O74" s="69" t="s">
         <v>355</v>
       </c>
-      <c r="P74" s="77" t="s">
+      <c r="P74" s="69" t="s">
         <v>355</v>
       </c>
       <c r="Q74" s="44"/>
@@ -8344,25 +9575,25 @@
       <c r="A75" s="44"/>
       <c r="B75" s="44"/>
       <c r="C75" s="44"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="80" t="s">
+      <c r="D75" s="80"/>
+      <c r="E75" s="86" t="s">
         <v>458</v>
       </c>
-      <c r="F75" s="81" t="s">
+      <c r="F75" s="72" t="s">
         <v>459</v>
       </c>
       <c r="G75" s="44"/>
       <c r="H75" s="44"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="76"/>
+      <c r="I75" s="84"/>
+      <c r="J75" s="85"/>
       <c r="K75" s="44"/>
       <c r="L75" s="44"/>
-      <c r="M75" s="72"/>
+      <c r="M75" s="80"/>
       <c r="N75" s="44"/>
-      <c r="O75" s="77" t="s">
+      <c r="O75" s="69" t="s">
         <v>362</v>
       </c>
-      <c r="P75" s="77" t="s">
+      <c r="P75" s="69" t="s">
         <v>362</v>
       </c>
       <c r="Q75" s="44"/>
@@ -8387,23 +9618,23 @@
       <c r="A76" s="44"/>
       <c r="B76" s="44"/>
       <c r="C76" s="44"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="80"/>
-      <c r="F76" s="74" t="s">
+      <c r="D76" s="80"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="68" t="s">
         <v>366</v>
       </c>
       <c r="G76" s="44"/>
       <c r="H76" s="44"/>
-      <c r="I76" s="75"/>
-      <c r="J76" s="76"/>
+      <c r="I76" s="84"/>
+      <c r="J76" s="85"/>
       <c r="K76" s="44"/>
       <c r="L76" s="44"/>
-      <c r="M76" s="72"/>
+      <c r="M76" s="80"/>
       <c r="N76" s="44"/>
-      <c r="O76" s="77" t="s">
+      <c r="O76" s="69" t="s">
         <v>366</v>
       </c>
-      <c r="P76" s="77" t="s">
+      <c r="P76" s="69" t="s">
         <v>366</v>
       </c>
       <c r="Q76" s="44"/>
@@ -8428,16 +9659,16 @@
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
       <c r="C77" s="44"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="73"/>
-      <c r="F77" s="73"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="67"/>
+      <c r="F77" s="67"/>
       <c r="G77" s="44"/>
       <c r="H77" s="44"/>
-      <c r="I77" s="82"/>
-      <c r="J77" s="76"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="85"/>
       <c r="K77" s="44"/>
       <c r="L77" s="44"/>
-      <c r="M77" s="72"/>
+      <c r="M77" s="80"/>
       <c r="N77" s="44"/>
       <c r="O77" s="44"/>
       <c r="P77" s="44"/>
@@ -8463,36 +9694,36 @@
       <c r="A78" s="44"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="74" t="s">
+      <c r="D78" s="80"/>
+      <c r="E78" s="68" t="s">
         <v>460</v>
       </c>
-      <c r="F78" s="81" t="s">
+      <c r="F78" s="72" t="s">
         <v>461</v>
       </c>
       <c r="G78" s="44"/>
       <c r="H78" s="44"/>
-      <c r="I78" s="83" t="s">
+      <c r="I78" s="74" t="s">
         <v>462</v>
       </c>
-      <c r="J78" s="76"/>
-      <c r="K78" s="77" t="s">
+      <c r="J78" s="85"/>
+      <c r="K78" s="69" t="s">
         <v>463</v>
       </c>
       <c r="L78" s="44"/>
-      <c r="M78" s="77" t="s">
+      <c r="M78" s="69" t="s">
         <v>464</v>
       </c>
-      <c r="N78" s="77" t="s">
+      <c r="N78" s="69" t="s">
         <v>465</v>
       </c>
-      <c r="O78" s="77" t="s">
+      <c r="O78" s="69" t="s">
         <v>466</v>
       </c>
-      <c r="P78" s="77" t="s">
+      <c r="P78" s="69" t="s">
         <v>466</v>
       </c>
-      <c r="Q78" s="77" t="s">
+      <c r="Q78" s="69" t="s">
         <v>467</v>
       </c>
       <c r="R78" s="44"/>
@@ -8516,28 +9747,28 @@
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="73"/>
-      <c r="F79" s="73"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="67"/>
+      <c r="F79" s="67"/>
       <c r="G79" s="44"/>
       <c r="H79" s="44"/>
-      <c r="I79" s="82"/>
-      <c r="J79" s="76"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="85"/>
       <c r="K79" s="44"/>
       <c r="L79" s="44"/>
-      <c r="M79" s="77" t="s">
+      <c r="M79" s="69" t="s">
         <v>468</v>
       </c>
-      <c r="N79" s="77" t="s">
+      <c r="N79" s="69" t="s">
         <v>469</v>
       </c>
-      <c r="O79" s="77" t="s">
+      <c r="O79" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="P79" s="77" t="s">
+      <c r="P79" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="Q79" s="79" t="s">
+      <c r="Q79" s="71" t="s">
         <v>470</v>
       </c>
       <c r="R79" s="44"/>
@@ -8561,22 +9792,22 @@
       <c r="A80" s="44"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="73"/>
-      <c r="F80" s="73"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="67"/>
+      <c r="F80" s="67"/>
       <c r="G80" s="44"/>
       <c r="H80" s="44"/>
-      <c r="I80" s="82"/>
-      <c r="J80" s="76"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="85"/>
       <c r="K80" s="44"/>
       <c r="L80" s="44"/>
-      <c r="M80" s="77" t="s">
+      <c r="M80" s="69" t="s">
         <v>471</v>
       </c>
-      <c r="N80" s="84" t="s">
+      <c r="N80" s="79" t="s">
         <v>472</v>
       </c>
-      <c r="O80" s="84"/>
+      <c r="O80" s="79"/>
       <c r="P80" s="44"/>
       <c r="Q80" s="44"/>
       <c r="R80" s="44"/>
@@ -8600,27 +9831,27 @@
       <c r="A81" s="44"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="85" t="s">
+      <c r="D81" s="80"/>
+      <c r="E81" s="78" t="s">
         <v>473</v>
       </c>
-      <c r="F81" s="85"/>
+      <c r="F81" s="78"/>
       <c r="G81" s="44"/>
       <c r="H81" s="44"/>
-      <c r="I81" s="83" t="s">
+      <c r="I81" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="J81" s="76"/>
+      <c r="J81" s="85"/>
       <c r="K81" s="44"/>
       <c r="L81" s="44"/>
-      <c r="M81" s="79" t="s">
+      <c r="M81" s="71" t="s">
         <v>474</v>
       </c>
       <c r="N81" s="44"/>
-      <c r="O81" s="77" t="s">
+      <c r="O81" s="69" t="s">
         <v>475</v>
       </c>
-      <c r="P81" s="77" t="s">
+      <c r="P81" s="69" t="s">
         <v>475</v>
       </c>
       <c r="Q81" s="44"/>
@@ -8654,10 +9885,10 @@
       <c r="J82" s="44"/>
       <c r="K82" s="44"/>
       <c r="L82" s="44"/>
-      <c r="M82" s="84" t="s">
+      <c r="M82" s="79" t="s">
         <v>476</v>
       </c>
-      <c r="N82" s="84"/>
+      <c r="N82" s="79"/>
       <c r="O82" s="44"/>
       <c r="P82" s="44"/>
       <c r="Q82" s="44"/>
@@ -8682,10 +9913,10 @@
       <c r="A83" s="44"/>
       <c r="B83" s="44"/>
       <c r="C83" s="44"/>
-      <c r="D83" s="72" t="s">
+      <c r="D83" s="80" t="s">
         <v>477</v>
       </c>
-      <c r="E83" s="77" t="s">
+      <c r="E83" s="69" t="s">
         <v>478</v>
       </c>
       <c r="F83" s="44"/>
@@ -8721,8 +9952,8 @@
       <c r="A84" s="44"/>
       <c r="B84" s="44"/>
       <c r="C84" s="44"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="79" t="s">
+      <c r="D84" s="80"/>
+      <c r="E84" s="71" t="s">
         <v>479</v>
       </c>
       <c r="F84" s="44"/>
@@ -8758,14 +9989,14 @@
       <c r="A85" s="44"/>
       <c r="B85" s="44"/>
       <c r="C85" s="44"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="77" t="s">
+      <c r="D85" s="80"/>
+      <c r="E85" s="69" t="s">
         <v>480</v>
       </c>
-      <c r="F85" s="77" t="s">
+      <c r="F85" s="69" t="s">
         <v>481</v>
       </c>
-      <c r="G85" s="77" t="s">
+      <c r="G85" s="69" t="s">
         <v>389</v>
       </c>
       <c r="H85" s="44"/>
@@ -8773,14 +10004,14 @@
       <c r="J85" s="44"/>
       <c r="K85" s="44"/>
       <c r="L85" s="44"/>
-      <c r="M85" s="77" t="s">
+      <c r="M85" s="69" t="s">
         <v>482</v>
       </c>
       <c r="N85" s="44"/>
-      <c r="O85" s="77" t="s">
+      <c r="O85" s="69" t="s">
         <v>483</v>
       </c>
-      <c r="P85" s="77" t="s">
+      <c r="P85" s="69" t="s">
         <v>483</v>
       </c>
       <c r="Q85" s="44"/>
@@ -8805,8 +10036,8 @@
       <c r="A86" s="44"/>
       <c r="B86" s="44"/>
       <c r="C86" s="44"/>
-      <c r="D86" s="72"/>
-      <c r="E86" s="79" t="s">
+      <c r="D86" s="80"/>
+      <c r="E86" s="71" t="s">
         <v>484</v>
       </c>
       <c r="F86" s="44"/>
@@ -8818,10 +10049,10 @@
       <c r="L86" s="44"/>
       <c r="M86" s="44"/>
       <c r="N86" s="44"/>
-      <c r="O86" s="77" t="s">
+      <c r="O86" s="69" t="s">
         <v>485</v>
       </c>
-      <c r="P86" s="77" t="s">
+      <c r="P86" s="69" t="s">
         <v>486</v>
       </c>
       <c r="Q86" s="44"/>
@@ -8857,10 +10088,10 @@
       <c r="L87" s="44"/>
       <c r="M87" s="44"/>
       <c r="N87" s="44"/>
-      <c r="O87" s="77" t="s">
+      <c r="O87" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="P87" s="79" t="s">
+      <c r="P87" s="71" t="s">
         <v>487</v>
       </c>
       <c r="Q87" s="44"/>
@@ -8890,7 +10121,7 @@
       <c r="F88" s="44"/>
       <c r="G88" s="44"/>
       <c r="H88" s="44"/>
-      <c r="I88" s="86" t="s">
+      <c r="I88" s="75" t="s">
         <v>488</v>
       </c>
       <c r="J88" s="44"/>
@@ -8898,10 +10129,10 @@
       <c r="L88" s="44"/>
       <c r="M88" s="44"/>
       <c r="N88" s="44"/>
-      <c r="O88" s="77" t="s">
+      <c r="O88" s="69" t="s">
         <v>489</v>
       </c>
-      <c r="P88" s="77" t="s">
+      <c r="P88" s="69" t="s">
         <v>489</v>
       </c>
       <c r="Q88" s="44"/>
@@ -9001,13 +10232,13 @@
       <c r="F91" s="44"/>
       <c r="G91" s="44"/>
       <c r="H91" s="44"/>
-      <c r="I91" s="86" t="s">
+      <c r="I91" s="75" t="s">
         <v>490</v>
       </c>
-      <c r="J91" s="77" t="s">
+      <c r="J91" s="69" t="s">
         <v>491</v>
       </c>
-      <c r="K91" s="77" t="s">
+      <c r="K91" s="69" t="s">
         <v>452</v>
       </c>
       <c r="L91" s="44"/>
@@ -40875,6 +42106,659 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="13" width="3.625" customWidth="1"/>
+    <col min="15" max="18" width="5.625" style="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="92" t="s">
+        <v>493</v>
+      </c>
+      <c r="G2" s="89"/>
+      <c r="H2" s="88" t="s">
+        <v>509</v>
+      </c>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88" t="s">
+        <v>508</v>
+      </c>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="O2" s="51" t="s">
+        <v>495</v>
+      </c>
+      <c r="P2" s="51">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="51">
+        <v>2</v>
+      </c>
+      <c r="R2" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" t="s">
+        <v>494</v>
+      </c>
+      <c r="O3" s="51" t="s">
+        <v>496</v>
+      </c>
+      <c r="P3" s="51" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q3" s="51" t="s">
+        <v>498</v>
+      </c>
+      <c r="R3" s="51" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88" t="s">
+        <v>507</v>
+      </c>
+      <c r="M4" s="88"/>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="92" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88"/>
+      <c r="M13" s="88"/>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="88"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="92" t="s">
+        <v>493</v>
+      </c>
+      <c r="G18" s="89"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="O18" s="51" t="s">
+        <v>495</v>
+      </c>
+      <c r="P18" s="51">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="51">
+        <v>2</v>
+      </c>
+      <c r="R18" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" t="s">
+        <v>503</v>
+      </c>
+      <c r="O19" s="51" t="s">
+        <v>496</v>
+      </c>
+      <c r="P19" s="93" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q19" s="93" t="s">
+        <v>501</v>
+      </c>
+      <c r="R19" s="93" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="88"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="88"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="B22" s="88"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="92" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+    </row>
+    <row r="26" spans="2:18">
+      <c r="B26" s="88"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18">
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+    </row>
+    <row r="28" spans="2:18">
+      <c r="B28" s="88"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="M28" s="88"/>
+    </row>
+    <row r="29" spans="2:18">
+      <c r="B29" s="88"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="88"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="88" t="s">
+        <v>505</v>
+      </c>
+      <c r="L29" s="88"/>
+      <c r="M29" s="88"/>
+    </row>
+    <row r="30" spans="2:18">
+      <c r="B30" s="88"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+    </row>
+    <row r="31" spans="2:18">
+      <c r="J31" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="88"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="92" t="s">
+        <v>493</v>
+      </c>
+      <c r="G35" s="89"/>
+      <c r="H35" s="88" t="s">
+        <v>510</v>
+      </c>
+      <c r="I35" s="88"/>
+      <c r="J35" s="88"/>
+      <c r="L35" s="88"/>
+      <c r="M35" s="88"/>
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" s="88"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="88"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88" t="s">
+        <v>511</v>
+      </c>
+      <c r="M36" s="88"/>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="88"/>
+      <c r="C37" s="88"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="88"/>
+      <c r="F37" s="88"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="88"/>
+      <c r="I37" s="88"/>
+      <c r="J37" s="88"/>
+      <c r="K37" s="88"/>
+      <c r="M37" s="88"/>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="88"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="88"/>
+      <c r="K38" s="88"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" s="88"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="88"/>
+      <c r="I39" s="88"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88" t="s">
+        <v>512</v>
+      </c>
+      <c r="M39" s="88"/>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" s="90"/>
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="90"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="90"/>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" s="88"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="88"/>
+      <c r="F41" s="88"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="88"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="92" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="88"/>
+      <c r="I42" s="88"/>
+      <c r="J42" s="88"/>
+      <c r="K42" s="88"/>
+      <c r="L42" s="88"/>
+      <c r="M42" s="88"/>
+    </row>
+    <row r="43" spans="2:13">
+      <c r="B43" s="88"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="88"/>
+      <c r="E43" s="88"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="88"/>
+      <c r="I43" s="88"/>
+      <c r="J43" s="88"/>
+      <c r="K43" s="88"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="88"/>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
+      <c r="F44" s="88"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="88"/>
+      <c r="I44" s="88"/>
+      <c r="J44" s="88"/>
+      <c r="K44" s="88"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="88"/>
+    </row>
+    <row r="45" spans="2:13">
+      <c r="B45" s="88"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="88"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+    </row>
+    <row r="46" spans="2:13">
+      <c r="B46" s="88"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
+      <c r="F46" s="88"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="88"/>
+      <c r="I46" s="88"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="88"/>
+    </row>
+    <row r="47" spans="2:13">
+      <c r="B47" s="88"/>
+      <c r="C47" s="88"/>
+      <c r="D47" s="88"/>
+      <c r="E47" s="88"/>
+      <c r="F47" s="88"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="88"/>
+      <c r="I47" s="88"/>
+      <c r="J47" s="88"/>
+      <c r="K47" s="88"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="88"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40961,7 +42845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D29"/>
   <sheetViews>
@@ -41113,7 +42997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C46"/>
   <sheetViews>
@@ -41343,7 +43227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I9"/>
   <sheetViews>
@@ -41395,7 +43279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D11"/>
   <sheetViews>
@@ -41463,674 +43347,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L149"/>
-  <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123:H124"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.75" customWidth="1"/>
-    <col min="8" max="8" width="9.625" customWidth="1"/>
-    <col min="12" max="12" width="11.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12">
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12">
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12">
-      <c r="B5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
-      <c r="E6" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="E7" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12">
-      <c r="K8" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="L8" s="33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
-      <c r="K9" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="L9" s="53"/>
-    </row>
-    <row r="12" spans="2:12">
-      <c r="B12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12">
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
-      <c r="B18" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="H18" t="s">
-        <v>116</v>
-      </c>
-      <c r="K18" t="s">
-        <v>117</v>
-      </c>
-      <c r="L18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" s="5" customFormat="1">
-      <c r="B24" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" s="5" customFormat="1">
-      <c r="B25" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" s="5" customFormat="1">
-      <c r="B26" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12">
-      <c r="B27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12">
-      <c r="B28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12">
-      <c r="B29" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12">
-      <c r="B30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12">
-      <c r="B31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12">
-      <c r="B32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12">
-      <c r="B51" s="37" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12">
-      <c r="B52" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12">
-      <c r="B53" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12">
-      <c r="B54" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12">
-      <c r="B56" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-    </row>
-    <row r="58" spans="2:12">
-      <c r="B58" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12">
-      <c r="B60" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12">
-      <c r="B61" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12">
-      <c r="B62" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12">
-      <c r="B64" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2">
-      <c r="B73" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" s="5" customFormat="1">
-      <c r="B76" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2">
-      <c r="B78" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2">
-      <c r="B79" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2">
-      <c r="B80" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2">
-      <c r="B84" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" s="5" customFormat="1">
-      <c r="B89" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2">
-      <c r="B90" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2">
-      <c r="B93" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2">
-      <c r="B94" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2">
-      <c r="B95" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2">
-      <c r="B96" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
-      <c r="B97" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2">
-      <c r="B98" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2">
-      <c r="B99" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2">
-      <c r="B100" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2">
-      <c r="B101" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2">
-      <c r="B102" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2">
-      <c r="B103" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2">
-      <c r="B104" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2">
-      <c r="B105" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2">
-      <c r="B106" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2">
-      <c r="B107" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2">
-      <c r="B108" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2">
-      <c r="B109" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2">
-      <c r="B110" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2">
-      <c r="B111" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" s="5" customFormat="1">
-      <c r="B113" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2">
-      <c r="B114" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2">
-      <c r="B115" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2">
-      <c r="B116" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2">
-      <c r="B117" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2">
-      <c r="B118" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2">
-      <c r="B119" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2">
-      <c r="B121" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2">
-      <c r="B122" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2">
-      <c r="B123" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2">
-      <c r="B124" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2">
-      <c r="B125" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2">
-      <c r="B126" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2">
-      <c r="B127" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2">
-      <c r="B128" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2">
-      <c r="B129" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2">
-      <c r="B130" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2">
-      <c r="B131" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2">
-      <c r="B132" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" s="5" customFormat="1">
-      <c r="B135" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2">
-      <c r="B136" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2">
-      <c r="B137" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2">
-      <c r="B138" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2">
-      <c r="B139" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2">
-      <c r="B140" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2">
-      <c r="B141" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2">
-      <c r="B142" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2">
-      <c r="B143" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2">
-      <c r="B144" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2">
-      <c r="B146" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2">
-      <c r="B147" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2">
-      <c r="B148" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2">
-      <c r="B149" t="s">
-        <v>271</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K9:L9"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>